<commit_message>
Step 3: Create shopping database and diagram
</commit_message>
<xml_diff>
--- a/A Lesson 16/B3. Build R diagram.xlsx
+++ b/A Lesson 16/B3. Build R diagram.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>MATHANG</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>GiaoHang</t>
-  </si>
-  <si>
-    <t>MaTT</t>
   </si>
   <si>
     <t>ThoiGian</t>
@@ -191,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +204,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -258,6 +267,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,11 +741,11 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
+      <c r="D20" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>31</v>
@@ -756,7 +767,7 @@
     </row>
     <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>9</v>
@@ -764,13 +775,17 @@
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>